<commit_message>
Logistica -> Distribucion -> Numero Guia
</commit_message>
<xml_diff>
--- a/public/templates/Template_NumeroGuia.xlsx
+++ b/public/templates/Template_NumeroGuia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndarRepositorys\PlataformaComercial\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2CBB950-CC77-4E9E-8273-A204A8B1E6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7A9F07-82D9-4FBB-9928-920C1A0EA86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7BFE7EE4-50B1-4D07-AE08-61DAB38FC954}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7BFE7EE4-50B1-4D07-AE08-61DAB38FC954}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Fletera</t>
   </si>
   <si>
     <t>Chofer</t>
-  </si>
-  <si>
-    <t>Importe Total</t>
   </si>
   <si>
     <t>Num. De Guia</t>
@@ -399,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2D7E96-9A18-46DD-9617-96358514226C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +408,7 @@
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,9 +416,6 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -434,13 +428,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7249BB-87F7-43E8-A73C-E1B4C295AF29}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>